<commit_message>
Added logo, social media icons
</commit_message>
<xml_diff>
--- a/Backup/Service.xlsx
+++ b/Backup/Service.xlsx
@@ -6,14 +6,14 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="test 640" r:id="rId3" sheetId="1"/>
-    <sheet name="test 7418" r:id="rId4" sheetId="2"/>
+    <sheet name="test 7418" r:id="rId3" sheetId="1"/>
+    <sheet name="test 640" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>Ημερομηνία</t>
   </si>
@@ -42,18 +42,42 @@
     <t>id</t>
   </si>
   <si>
+    <t>2019-10-30</t>
+  </si>
+  <si>
+    <t>Μικρό</t>
+  </si>
+  <si>
+    <t>Σκακι</t>
+  </si>
+  <si>
+    <t>Σπίτι</t>
+  </si>
+  <si>
+    <t>2020-10-30</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2019-10-22</t>
+  </si>
+  <si>
+    <t>Σσαδ</t>
+  </si>
+  <si>
+    <t>2020-10-22</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>2019-10-20</t>
   </si>
   <si>
-    <t>Μικρό</t>
-  </si>
-  <si>
     <t>Λάδια</t>
   </si>
   <si>
-    <t>Σπίτι</t>
-  </si>
-  <si>
     <t>2020-10-20</t>
   </si>
   <si>
@@ -73,42 +97,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>2020-10-07</t>
-  </si>
-  <si>
-    <t>Λάδια|Φίλτρα</t>
-  </si>
-  <si>
-    <t>2021-10-07</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>2019-10-30</t>
-  </si>
-  <si>
-    <t>Σκακι</t>
-  </si>
-  <si>
-    <t>2020-10-30</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>2019-10-22</t>
-  </si>
-  <si>
-    <t>Σσαδ</t>
-  </si>
-  <si>
-    <t>2020-10-22</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
 </sst>
 </file>
@@ -224,19 +212,19 @@
         <v>11</v>
       </c>
       <c r="D2" t="n">
-        <v>25000.0</v>
+        <v>150000.0</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>55000.0</v>
+        <v>210000.0</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="H2" t="n">
-        <v>250.0</v>
+        <v>355.0</v>
       </c>
       <c r="I2" t="s">
         <v>14</v>
@@ -247,28 +235,28 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" t="n">
-        <v>27.0</v>
+        <v>87000.0</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="n">
-        <v>30027.0</v>
+        <v>147000.0</v>
       </c>
       <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="I3" t="s">
         <v>18</v>
-      </c>
-      <c r="H3" t="n">
-        <v>500.0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -278,7 +266,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -286,7 +274,7 @@
   <cols>
     <col min="1" max="1" width="15.8359375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="8.53125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.0390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.1484375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="14.453125" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="13.17578125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="18.91796875" customWidth="true" bestFit="true"/>
@@ -326,89 +314,60 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>221500.0</v>
+        <v>25000.0</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="n">
-        <v>281500.0</v>
+        <v>55000.0</v>
       </c>
       <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="I2" t="s">
         <v>22</v>
-      </c>
-      <c r="H2" t="n">
-        <v>300.0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>25</v>
       </c>
       <c r="D3" t="n">
-        <v>150000.0</v>
+        <v>27.0</v>
       </c>
       <c r="E3" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="n">
-        <v>210000.0</v>
+        <v>30027.0</v>
       </c>
       <c r="G3" t="s">
         <v>26</v>
       </c>
       <c r="H3" t="n">
-        <v>355.0</v>
+        <v>500.0</v>
       </c>
       <c r="I3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="n">
-        <v>87000.0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="n">
-        <v>147000.0</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="n">
-        <v>250.0</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>